<commit_message>
added more data and graphs/results
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Data 1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>average wait time</t>
   </si>
@@ -43,14 +43,126 @@
   </si>
   <si>
     <t>altered downtime</t>
+  </si>
+  <si>
+    <t>total calls: 50</t>
+  </si>
+  <si>
+    <t>simulation stops after 24 hours</t>
+  </si>
+  <si>
+    <t>calls handled</t>
+  </si>
+  <si>
+    <r>
+      <t>italics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>means unsure</t>
+    </r>
+  </si>
+  <si>
+    <t>It seems that the total downtime is so close every time that the number of calls handled is never changed. However, the number of calls stacked up does change, resulting in a higher average wait time for more calls stacked up.</t>
+  </si>
+  <si>
+    <t>finishing queue</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>handled 47 calls!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calls incoming </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(calls handled always 46)</t>
+    </r>
+  </si>
+  <si>
+    <t>interesting to compare with the above</t>
+  </si>
+  <si>
+    <t>Most of the total downtime is at the beginning when waiting for first call to come in</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Mean waiting time</t>
+  </si>
+  <si>
+    <t>Max waiting time</t>
+  </si>
+  <si>
+    <t>Min waiting time</t>
+  </si>
+  <si>
+    <t>Mean downtime</t>
+  </si>
+  <si>
+    <t>Max downtime</t>
+  </si>
+  <si>
+    <t>Min downtime</t>
+  </si>
+  <si>
+    <t>Range waiting time</t>
+  </si>
+  <si>
+    <t>Range downtime</t>
+  </si>
+  <si>
+    <t>Median waiting time</t>
+  </si>
+  <si>
+    <t>Median downtime</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>The average waiting time generally increases as the program goes on (maybe make an average waiting time against time graph?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -74,12 +186,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -89,7 +273,1205 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>average wait time against</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>calls incoming</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>calls incoming against average wait time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data 2'!$E$11:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data 2'!$A$11:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="93537024"/>
+        <c:axId val="64126976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="93537024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>calls incoming</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="64126976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64126976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> wait time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93537024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>average wait time against total downtime</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data 2'!$C$2:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data 2'!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="95373952"/>
+        <c:axId val="100934400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="95373952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> downtime</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100934400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="100934400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> wait time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95373952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="1391" t="14844" r="54392" b="6510"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7239000" y="266699"/>
+          <a:ext cx="3000375" cy="3000375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>5630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10077449" y="1148630"/>
+          <a:ext cx="1200151" cy="1070695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>figure 4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>increase</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> then decrease in queue length</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2051" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect l="1391" t="14974" r="54392" b="6380"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11772899" y="266699"/>
+          <a:ext cx="3000375" cy="3000375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>167555</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13039724" y="1120055"/>
+          <a:ext cx="1200151" cy="1070695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>figure 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>lots of calls stacked up at the end</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>221494</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect l="659" t="13021" r="62298" b="21354"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14858999" y="257174"/>
+          <a:ext cx="3021845" cy="3009901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>43730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16125824" y="1186730"/>
+          <a:ext cx="1200151" cy="1156420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>figure 6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>three more</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> incoming calls per day than most makes a high queue</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2053" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect l="659" t="13021" r="62445" b="21354"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17973675" y="257175"/>
+          <a:ext cx="3009900" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>99145</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19297650" y="1228725"/>
+          <a:ext cx="1200151" cy="1156420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>figure 7</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>compare with figure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> 6...</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19583</cdr:x>
+      <cdr:y>0.36458</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="895350" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>graph</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t> 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>shows how calls incoming is very important</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01875</cdr:x>
+      <cdr:y>0.81944</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.21875</cdr:x>
+      <cdr:y>0.95486</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="85725" y="2247900"/>
+          <a:ext cx="914400" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19583</cdr:x>
+      <cdr:y>0.36458</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="895350" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>graph</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t> 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>shows how downtime isn't that important</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -712,10 +2094,537 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>0.39</v>
+      </c>
+      <c r="B2">
+        <v>18.3</v>
+      </c>
+      <c r="C2">
+        <v>0.75</v>
+      </c>
+      <c r="E2" s="2">
+        <v>46</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>0.13</v>
+      </c>
+      <c r="B3">
+        <v>6.15</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B4">
+        <v>12.95</v>
+      </c>
+      <c r="C4">
+        <v>0.65</v>
+      </c>
+      <c r="E4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>0.27</v>
+      </c>
+      <c r="B5">
+        <v>12.5</v>
+      </c>
+      <c r="C5">
+        <v>0.65</v>
+      </c>
+      <c r="E5">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>0.62</v>
+      </c>
+      <c r="B6">
+        <v>29.9</v>
+      </c>
+      <c r="C6">
+        <v>0.45</v>
+      </c>
+      <c r="E6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>0.54</v>
+      </c>
+      <c r="B7">
+        <v>26.5</v>
+      </c>
+      <c r="C7">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>0.69</v>
+      </c>
+      <c r="B8">
+        <v>33.9</v>
+      </c>
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>0.43</v>
+      </c>
+      <c r="B9">
+        <v>20.2</v>
+      </c>
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B11">
+        <v>12.95</v>
+      </c>
+      <c r="C11">
+        <v>0.6</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>0.79</v>
+      </c>
+      <c r="B12">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B13">
+        <v>28.15</v>
+      </c>
+      <c r="C13">
+        <v>0.4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B14">
+        <v>28.65</v>
+      </c>
+      <c r="C14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>0.36</v>
+      </c>
+      <c r="B15">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>0.25</v>
+      </c>
+      <c r="B16">
+        <v>12.1</v>
+      </c>
+      <c r="C16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>0.25</v>
+      </c>
+      <c r="B17">
+        <v>11.75</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A18">
+        <v>0.32</v>
+      </c>
+      <c r="B18">
+        <v>15.5</v>
+      </c>
+      <c r="C18">
+        <v>0.65</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>0.36</v>
+      </c>
+      <c r="B19">
+        <v>17.8</v>
+      </c>
+      <c r="C19">
+        <v>0.65</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="M19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>0.43</v>
+      </c>
+      <c r="B20">
+        <v>21.3</v>
+      </c>
+      <c r="C20">
+        <v>0.4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>48</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="7">
+        <f>AVERAGE(A2:A53)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="M20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>0.39</v>
+      </c>
+      <c r="B21">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.6</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>47</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="7">
+        <f>MEDIAN(A2:A50)</f>
+        <v>0.39</v>
+      </c>
+      <c r="M21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>0.82</v>
+      </c>
+      <c r="B22">
+        <v>40.9</v>
+      </c>
+      <c r="C22">
+        <v>0.4</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>49</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="7">
+        <f>MAX(A2:A53)</f>
+        <v>0.82</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="H23" s="3"/>
+      <c r="I23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="7">
+        <f>MIN(A2:A53)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="I24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="7">
+        <f>J22-J23</f>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="I26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="7">
+        <f>AVERAGE(C2:C53)</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="I27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="7">
+        <f>MEDIAN(C2:C50)</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="I28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="7">
+        <f>MAX(C2:C53)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="I29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="7">
+        <f>MIN(C2:C53)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1">
+      <c r="I30" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="10">
+        <f>J28-J29</f>
+        <v>0.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15"/>
@@ -730,22 +2639,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
@@ -790,6 +2699,9 @@
         <f t="shared" ref="E3:E22" si="0">(29-D3) + C3</f>
         <v>3.9500000000000015</v>
       </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
@@ -986,18 +2898,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
uploaded images and edited presentation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>average wait time</t>
   </si>
@@ -142,6 +142,12 @@
       </rPr>
       <t>(calls handled usually 46)</t>
     </r>
+  </si>
+  <si>
+    <t>altered downtime = 29 - time end + total downtime</t>
+  </si>
+  <si>
+    <t>29 is arbitrary</t>
   </si>
 </sst>
 </file>
@@ -591,12 +597,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="48119808"/>
-        <c:axId val="48121728"/>
+        <c:axId val="64901120"/>
+        <c:axId val="64903040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48119808"/>
+        <c:axId val="64901120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,12 +626,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48121728"/>
+        <c:crossAx val="64903040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48121728"/>
+        <c:axId val="64903040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +662,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48119808"/>
+        <c:crossAx val="64901120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -667,7 +672,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1003,12 +1008,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="48135168"/>
-        <c:axId val="48489216"/>
+        <c:axId val="64923904"/>
+        <c:axId val="64970752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48135168"/>
+        <c:axId val="64923904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1039,12 +1043,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48489216"/>
+        <c:crossAx val="64970752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48489216"/>
+        <c:axId val="64970752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1079,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48135168"/>
+        <c:crossAx val="64923904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,7 +1089,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1376,11 +1380,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="57191040"/>
-        <c:axId val="57189504"/>
+        <c:axId val="66462080"/>
+        <c:axId val="66464000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57191040"/>
+        <c:axId val="66462080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,12 +1409,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57189504"/>
+        <c:crossAx val="66464000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57189504"/>
+        <c:axId val="66464000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,7 +1440,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57191040"/>
+        <c:crossAx val="66462080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1445,7 +1449,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2455,10 +2459,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1447800" cy="981075"/>
     <xdr:sp macro="" textlink="">
@@ -2468,7 +2472,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6524625" y="1447799"/>
+          <a:off x="6943725" y="1428749"/>
           <a:ext cx="1447800" cy="981075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2502,7 +2506,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> if their downtime is less than or equal to 4</a:t>
+            <a:t> if their downtime is less than or equal to 4 (in green)</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -3380,8 +3384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H32" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4374,10 +4378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15"/>
@@ -4386,7 +4390,7 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4575,10 +4579,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
+        <v>0.23</v>
+      </c>
+      <c r="B10">
         <v>11.95</v>
-      </c>
-      <c r="B10">
-        <v>0.23</v>
       </c>
       <c r="C10">
         <v>0.6</v>
@@ -4646,6 +4650,16 @@
       </c>
       <c r="F13">
         <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="C16" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>